<commit_message>
Eliminate inefficiencies in some examples
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/testConferenceSchedulingConstraints.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/testConferenceSchedulingConstraints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="56"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -980,10 +980,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C27" activeCellId="1" sqref="B1 C27"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -1431,7 +1431,7 @@
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1640,7 +1640,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1832,7 +1832,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2025,7 +2025,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2217,7 +2217,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2234,12 +2234,12 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2309,7 +2309,7 @@
         <v>171</v>
       </c>
       <c r="B4" s="12" t="n">
-        <v>-60</v>
+        <v>-120</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -2409,7 +2409,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2604,7 +2604,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2813,7 +2813,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3024,7 +3024,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3237,7 +3237,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3438,7 +3438,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3459,10 +3459,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" activeCellId="1" sqref="B1 D18"/>
+      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.08"/>
@@ -3590,7 +3590,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3785,7 +3785,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3980,7 +3980,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4177,7 +4177,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4387,7 +4387,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4598,7 +4598,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4811,7 +4811,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5029,7 +5029,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5257,7 +5257,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5468,7 +5468,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5679,7 +5679,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5700,10 +5700,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E17" activeCellId="1" sqref="B1 E17"/>
+      <selection pane="bottomRight" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
@@ -5867,7 +5867,7 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6095,7 +6095,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6306,7 +6306,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6529,7 +6529,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6752,7 +6752,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6971,7 +6971,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7194,7 +7194,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7421,7 +7421,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7634,7 +7634,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7847,7 +7847,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8060,7 +8060,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8081,10 +8081,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="1" sqref="B1 A7"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.7"/>
@@ -8261,7 +8261,7 @@
     <mergeCell ref="N1:P1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8474,7 +8474,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8687,7 +8687,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8900,7 +8900,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9115,7 +9115,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9330,7 +9330,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9545,7 +9545,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9760,7 +9760,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9983,7 +9983,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10178,7 +10178,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10377,7 +10377,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10398,10 +10398,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" activeCellId="1" sqref="B1 A11"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.95"/>
@@ -12509,7 +12509,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -12708,7 +12708,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -12907,7 +12907,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13106,7 +13106,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13298,7 +13298,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13509,7 +13509,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13720,7 +13720,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13931,7 +13931,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13948,7 +13948,7 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -14142,7 +14142,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14335,7 +14335,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14527,7 +14527,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14722,7 +14722,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14916,7 +14916,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
Improve performance of some examples (#2137)
* Eliminate inefficiencies in some examples

* Further updates to examples

* Fix tests

* Remove a hackish change
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/testConferenceSchedulingConstraints.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/testConferenceSchedulingConstraints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="56"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -980,10 +980,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C27" activeCellId="1" sqref="B1 C27"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -1431,7 +1431,7 @@
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1640,7 +1640,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1832,7 +1832,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2025,7 +2025,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2217,7 +2217,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2234,12 +2234,12 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2309,7 +2309,7 @@
         <v>171</v>
       </c>
       <c r="B4" s="12" t="n">
-        <v>-60</v>
+        <v>-120</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -2409,7 +2409,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2604,7 +2604,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2813,7 +2813,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3024,7 +3024,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3237,7 +3237,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3438,7 +3438,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3459,10 +3459,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" activeCellId="1" sqref="B1 D18"/>
+      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.08"/>
@@ -3590,7 +3590,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3785,7 +3785,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3980,7 +3980,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4177,7 +4177,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4387,7 +4387,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4598,7 +4598,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -4811,7 +4811,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5029,7 +5029,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5257,7 +5257,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5468,7 +5468,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5679,7 +5679,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -5700,10 +5700,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E17" activeCellId="1" sqref="B1 E17"/>
+      <selection pane="bottomRight" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
@@ -5867,7 +5867,7 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6095,7 +6095,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6306,7 +6306,7 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6529,7 +6529,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6752,7 +6752,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6971,7 +6971,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7194,7 +7194,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7421,7 +7421,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7634,7 +7634,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -7847,7 +7847,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8060,7 +8060,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8081,10 +8081,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="1" sqref="B1 A7"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.7"/>
@@ -8261,7 +8261,7 @@
     <mergeCell ref="N1:P1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8474,7 +8474,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8687,7 +8687,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -8900,7 +8900,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9115,7 +9115,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9330,7 +9330,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9545,7 +9545,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9760,7 +9760,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -9983,7 +9983,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10178,7 +10178,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10377,7 +10377,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -10398,10 +10398,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" activeCellId="1" sqref="B1 A11"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.95"/>
@@ -12509,7 +12509,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -12708,7 +12708,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -12907,7 +12907,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13106,7 +13106,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13298,7 +13298,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13509,7 +13509,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13720,7 +13720,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13931,7 +13931,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -13948,7 +13948,7 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -14142,7 +14142,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14335,7 +14335,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14527,7 +14527,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14722,7 +14722,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -14916,7 +14916,7 @@
     <mergeCell ref="B6:D6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>